<commit_message>
update for Matz lab
</commit_message>
<xml_diff>
--- a/troubleshoot_ids/barcoding_plates_GD_5-1-20.xlsx
+++ b/troubleshoot_ids/barcoding_plates_GD_5-1-20.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/grovesdixon/gitreps/stick_switching/troubleshoot_ids/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{3BCB907D-8451-8741-ABE5-6E0B6D8F6EBF}" xr6:coauthVersionLast="36" xr6:coauthVersionMax="36" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{E5B2AA67-3370-5943-A401-694504F8F33D}" xr6:coauthVersionLast="36" xr6:coauthVersionMax="36" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="4420" yWindow="2380" windowWidth="34280" windowHeight="19260" activeTab="1" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="380" yWindow="1000" windowWidth="25000" windowHeight="19260" activeTab="1" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="original" sheetId="1" r:id="rId1"/>
@@ -115,7 +115,7 @@
       <scheme val="minor"/>
     </font>
   </fonts>
-  <fills count="6">
+  <fills count="7">
     <fill>
       <patternFill patternType="none"/>
     </fill>
@@ -146,6 +146,12 @@
         <bgColor indexed="64"/>
       </patternFill>
     </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="6"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
   </fills>
   <borders count="1">
     <border>
@@ -159,7 +165,7 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="14">
+  <cellXfs count="19">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1"/>
     <xf numFmtId="0" fontId="0" fillId="2" borderId="0" xfId="0" applyFill="1"/>
@@ -183,14 +189,29 @@
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment horizontal="right"/>
     </xf>
-    <xf numFmtId="0" fontId="1" fillId="4" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
-      <alignment horizontal="right"/>
-    </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFill="1" applyAlignment="1">
       <alignment horizontal="right"/>
     </xf>
     <xf numFmtId="0" fontId="1" fillId="5" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
       <alignment horizontal="right"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="3" borderId="0" xfId="0" applyFill="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="6" borderId="0" xfId="0" applyFill="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
+      <alignment horizontal="right"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFill="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="3" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="6" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
+      <alignment horizontal="center"/>
     </xf>
   </cellXfs>
   <cellStyles count="1">
@@ -1716,8 +1737,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{6657578F-71EC-C847-9B2C-95C15CFFFAF1}">
   <dimension ref="A1:AC47"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A8" workbookViewId="0">
-      <selection activeCell="S14" sqref="S14"/>
+    <sheetView tabSelected="1" topLeftCell="A15" workbookViewId="0">
+      <selection activeCell="O51" sqref="O51"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="11" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
@@ -2658,22 +2679,22 @@
       <c r="S27" s="8">
         <v>80</v>
       </c>
-      <c r="T27" s="13">
+      <c r="T27" s="12">
         <v>72</v>
       </c>
       <c r="U27" s="10">
         <v>64</v>
       </c>
-      <c r="V27" s="13">
+      <c r="V27" s="12">
         <v>56</v>
       </c>
-      <c r="W27" s="12">
+      <c r="W27" s="11">
         <v>48</v>
       </c>
-      <c r="X27" s="12">
+      <c r="X27" s="11">
         <v>40</v>
       </c>
-      <c r="Y27" s="12">
+      <c r="Y27" s="11">
         <v>32</v>
       </c>
       <c r="Z27" s="8">
@@ -2693,7 +2714,7 @@
       <c r="A28" s="2" t="s">
         <v>2</v>
       </c>
-      <c r="B28">
+      <c r="B28" s="3">
         <v>2</v>
       </c>
       <c r="C28">
@@ -2744,22 +2765,22 @@
       <c r="S28" s="8">
         <v>79</v>
       </c>
-      <c r="T28" s="13">
+      <c r="T28" s="12">
         <v>71</v>
       </c>
       <c r="U28" s="10">
         <v>63</v>
       </c>
-      <c r="V28" s="13">
+      <c r="V28" s="12">
         <v>55</v>
       </c>
-      <c r="W28" s="12">
+      <c r="W28" s="11">
         <v>47</v>
       </c>
-      <c r="X28" s="12">
+      <c r="X28" s="11">
         <v>39</v>
       </c>
-      <c r="Y28" s="12">
+      <c r="Y28" s="11">
         <v>31</v>
       </c>
       <c r="Z28" s="8">
@@ -2779,7 +2800,7 @@
       <c r="A29" s="2" t="s">
         <v>3</v>
       </c>
-      <c r="B29">
+      <c r="B29" s="3">
         <v>3</v>
       </c>
       <c r="C29">
@@ -2833,19 +2854,19 @@
       <c r="T29" s="10">
         <v>70</v>
       </c>
-      <c r="U29" s="13">
+      <c r="U29" s="12">
         <v>62</v>
       </c>
-      <c r="V29" s="13">
+      <c r="V29" s="12">
         <v>54</v>
       </c>
-      <c r="W29" s="12">
+      <c r="W29" s="11">
         <v>46</v>
       </c>
-      <c r="X29" s="12">
+      <c r="X29" s="11">
         <v>38</v>
       </c>
-      <c r="Y29" s="12">
+      <c r="Y29" s="11">
         <v>30</v>
       </c>
       <c r="Z29" s="8">
@@ -2919,19 +2940,19 @@
       <c r="T30" s="10">
         <v>69</v>
       </c>
-      <c r="U30" s="13">
+      <c r="U30" s="12">
         <v>61</v>
       </c>
-      <c r="V30" s="13">
+      <c r="V30" s="12">
         <v>53</v>
       </c>
-      <c r="W30" s="12">
+      <c r="W30" s="11">
         <v>45</v>
       </c>
-      <c r="X30" s="12">
+      <c r="X30" s="11">
         <v>37</v>
       </c>
-      <c r="Y30" s="12">
+      <c r="Y30" s="11">
         <v>29</v>
       </c>
       <c r="Z30" s="8">
@@ -3002,22 +3023,22 @@
       <c r="S31" s="8">
         <v>76</v>
       </c>
-      <c r="T31" s="13">
+      <c r="T31" s="12">
         <v>68</v>
       </c>
-      <c r="U31" s="13">
+      <c r="U31" s="12">
         <v>60</v>
       </c>
       <c r="V31" s="10">
         <v>52</v>
       </c>
-      <c r="W31" s="12">
+      <c r="W31" s="11">
         <v>44</v>
       </c>
-      <c r="X31" s="12">
+      <c r="X31" s="11">
         <v>36</v>
       </c>
-      <c r="Y31" s="12">
+      <c r="Y31" s="11">
         <v>28</v>
       </c>
       <c r="Z31" s="8">
@@ -3070,7 +3091,7 @@
       <c r="L32">
         <v>86</v>
       </c>
-      <c r="M32">
+      <c r="M32" s="3">
         <v>94</v>
       </c>
       <c r="N32" t="s">
@@ -3088,22 +3109,22 @@
       <c r="S32" s="8">
         <v>75</v>
       </c>
-      <c r="T32" s="13">
+      <c r="T32" s="12">
         <v>67</v>
       </c>
-      <c r="U32" s="13">
+      <c r="U32" s="12">
         <v>59</v>
       </c>
       <c r="V32" s="10">
         <v>51</v>
       </c>
-      <c r="W32" s="12">
+      <c r="W32" s="11">
         <v>43</v>
       </c>
-      <c r="X32" s="12">
+      <c r="X32" s="11">
         <v>35</v>
       </c>
-      <c r="Y32" s="12">
+      <c r="Y32" s="11">
         <v>27</v>
       </c>
       <c r="Z32" s="8">
@@ -3156,7 +3177,7 @@
       <c r="L33">
         <v>87</v>
       </c>
-      <c r="M33">
+      <c r="M33" s="3">
         <v>95</v>
       </c>
       <c r="N33" t="s">
@@ -3174,22 +3195,22 @@
       <c r="S33" s="8">
         <v>74</v>
       </c>
-      <c r="T33" s="13">
+      <c r="T33" s="12">
         <v>66</v>
       </c>
       <c r="U33" s="10">
         <v>58</v>
       </c>
-      <c r="V33" s="13">
+      <c r="V33" s="12">
         <v>50</v>
       </c>
-      <c r="W33" s="12">
+      <c r="W33" s="11">
         <v>42</v>
       </c>
-      <c r="X33" s="12">
+      <c r="X33" s="11">
         <v>34</v>
       </c>
-      <c r="Y33" s="12">
+      <c r="Y33" s="11">
         <v>26</v>
       </c>
       <c r="Z33" s="8">
@@ -3260,22 +3281,22 @@
       <c r="S34" s="8">
         <v>73</v>
       </c>
-      <c r="T34" s="13">
+      <c r="T34" s="12">
         <v>65</v>
       </c>
       <c r="U34" s="10">
         <v>57</v>
       </c>
-      <c r="V34" s="13">
+      <c r="V34" s="12">
         <v>49</v>
       </c>
-      <c r="W34" s="12">
+      <c r="W34" s="11">
         <v>41</v>
       </c>
-      <c r="X34" s="12">
+      <c r="X34" s="11">
         <v>33</v>
       </c>
-      <c r="Y34" s="12">
+      <c r="Y34" s="11">
         <v>25</v>
       </c>
       <c r="Z34" s="8">
@@ -3379,40 +3400,40 @@
       <c r="A40" s="2" t="s">
         <v>1</v>
       </c>
-      <c r="B40" s="5" t="s">
+      <c r="B40" s="7" t="s">
         <v>17</v>
       </c>
       <c r="C40" s="5" t="s">
         <v>18</v>
       </c>
-      <c r="D40" s="5" t="s">
-        <v>19</v>
-      </c>
-      <c r="E40" s="5" t="s">
+      <c r="D40" s="7" t="s">
+        <v>19</v>
+      </c>
+      <c r="E40" s="18" t="s">
         <v>17</v>
       </c>
       <c r="F40" s="5" t="s">
         <v>18</v>
       </c>
-      <c r="G40" s="5" t="s">
-        <v>19</v>
-      </c>
-      <c r="H40" s="5" t="s">
+      <c r="G40" s="18" t="s">
+        <v>19</v>
+      </c>
+      <c r="H40" s="7" t="s">
         <v>17</v>
       </c>
       <c r="I40" s="5" t="s">
         <v>18</v>
       </c>
-      <c r="J40" s="5" t="s">
-        <v>19</v>
-      </c>
-      <c r="K40" s="5" t="s">
+      <c r="J40" s="7" t="s">
+        <v>19</v>
+      </c>
+      <c r="K40" s="7" t="s">
         <v>17</v>
       </c>
       <c r="L40" s="5" t="s">
         <v>18</v>
       </c>
-      <c r="M40" s="5" t="s">
+      <c r="M40" s="7" t="s">
         <v>17</v>
       </c>
       <c r="P40" s="2" t="s">
@@ -3436,13 +3457,13 @@
       <c r="V40" s="9" t="s">
         <v>17</v>
       </c>
-      <c r="W40" s="11" t="s">
-        <v>19</v>
-      </c>
-      <c r="X40" s="5" t="s">
-        <v>18</v>
-      </c>
-      <c r="Y40" s="11" t="s">
+      <c r="W40" s="15" t="s">
+        <v>19</v>
+      </c>
+      <c r="X40" s="16" t="s">
+        <v>18</v>
+      </c>
+      <c r="Y40" s="15" t="s">
         <v>17</v>
       </c>
       <c r="Z40" s="7" t="s">
@@ -3459,46 +3480,46 @@
       <c r="A41" s="2" t="s">
         <v>2</v>
       </c>
-      <c r="B41" s="5" t="s">
+      <c r="B41" s="14" t="s">
         <v>18</v>
       </c>
       <c r="C41" s="5" t="s">
         <v>18</v>
       </c>
-      <c r="D41" s="5" t="s">
-        <v>19</v>
-      </c>
-      <c r="E41" s="5" t="s">
+      <c r="D41" s="7" t="s">
+        <v>19</v>
+      </c>
+      <c r="E41" s="18" t="s">
         <v>17</v>
       </c>
       <c r="F41" s="5" t="s">
         <v>18</v>
       </c>
-      <c r="G41" s="5" t="s">
-        <v>19</v>
-      </c>
-      <c r="H41" s="5" t="s">
+      <c r="G41" s="18" t="s">
+        <v>19</v>
+      </c>
+      <c r="H41" s="7" t="s">
         <v>17</v>
       </c>
       <c r="I41" s="5" t="s">
         <v>18</v>
       </c>
-      <c r="J41" s="5" t="s">
-        <v>19</v>
-      </c>
-      <c r="K41" s="5" t="s">
+      <c r="J41" s="7" t="s">
+        <v>19</v>
+      </c>
+      <c r="K41" s="7" t="s">
         <v>17</v>
       </c>
       <c r="L41" s="5" t="s">
         <v>18</v>
       </c>
-      <c r="M41" s="5" t="s">
+      <c r="M41" s="7" t="s">
         <v>17</v>
       </c>
       <c r="P41" s="2" t="s">
         <v>2</v>
       </c>
-      <c r="Q41" s="5" t="s">
+      <c r="Q41" s="17" t="s">
         <v>19</v>
       </c>
       <c r="R41" s="5" t="s">
@@ -3516,13 +3537,13 @@
       <c r="V41" s="9" t="s">
         <v>17</v>
       </c>
-      <c r="W41" s="11" t="s">
-        <v>19</v>
-      </c>
-      <c r="X41" s="5" t="s">
-        <v>18</v>
-      </c>
-      <c r="Y41" s="11" t="s">
+      <c r="W41" s="15" t="s">
+        <v>19</v>
+      </c>
+      <c r="X41" s="16" t="s">
+        <v>18</v>
+      </c>
+      <c r="Y41" s="15" t="s">
         <v>17</v>
       </c>
       <c r="Z41" s="7" t="s">
@@ -3539,46 +3560,46 @@
       <c r="A42" s="2" t="s">
         <v>3</v>
       </c>
-      <c r="B42" s="5" t="s">
-        <v>17</v>
-      </c>
-      <c r="C42" s="5" t="s">
-        <v>17</v>
-      </c>
-      <c r="D42" s="5" t="s">
+      <c r="B42" s="14" t="s">
+        <v>17</v>
+      </c>
+      <c r="C42" s="7" t="s">
+        <v>17</v>
+      </c>
+      <c r="D42" s="7" t="s">
         <v>17</v>
       </c>
       <c r="E42" s="5" t="s">
         <v>18</v>
       </c>
-      <c r="F42" s="5" t="s">
-        <v>19</v>
-      </c>
-      <c r="G42" s="5" t="s">
+      <c r="F42" s="18" t="s">
+        <v>19</v>
+      </c>
+      <c r="G42" s="18" t="s">
         <v>17</v>
       </c>
       <c r="H42" s="5" t="s">
         <v>18</v>
       </c>
-      <c r="I42" s="5" t="s">
-        <v>19</v>
-      </c>
-      <c r="J42" s="5" t="s">
+      <c r="I42" s="7" t="s">
+        <v>19</v>
+      </c>
+      <c r="J42" s="7" t="s">
         <v>17</v>
       </c>
       <c r="K42" s="5" t="s">
         <v>18</v>
       </c>
-      <c r="L42" s="5" t="s">
-        <v>19</v>
-      </c>
-      <c r="M42" s="5" t="s">
+      <c r="L42" s="7" t="s">
+        <v>19</v>
+      </c>
+      <c r="M42" s="7" t="s">
         <v>17</v>
       </c>
       <c r="P42" s="2" t="s">
         <v>3</v>
       </c>
-      <c r="Q42" s="7" t="s">
+      <c r="Q42" s="13" t="s">
         <v>18</v>
       </c>
       <c r="R42" s="7" t="s">
@@ -3596,13 +3617,13 @@
       <c r="V42" s="9" t="s">
         <v>19</v>
       </c>
-      <c r="W42" s="5" t="s">
-        <v>18</v>
-      </c>
-      <c r="X42" s="11" t="s">
-        <v>17</v>
-      </c>
-      <c r="Y42" s="11" t="s">
+      <c r="W42" s="16" t="s">
+        <v>18</v>
+      </c>
+      <c r="X42" s="15" t="s">
+        <v>17</v>
+      </c>
+      <c r="Y42" s="15" t="s">
         <v>19</v>
       </c>
       <c r="Z42" s="5" t="s">
@@ -3622,37 +3643,37 @@
       <c r="B43" s="5" t="s">
         <v>18</v>
       </c>
-      <c r="C43" s="5" t="s">
-        <v>17</v>
-      </c>
-      <c r="D43" s="5" t="s">
+      <c r="C43" s="7" t="s">
+        <v>17</v>
+      </c>
+      <c r="D43" s="7" t="s">
         <v>17</v>
       </c>
       <c r="E43" s="5" t="s">
         <v>18</v>
       </c>
-      <c r="F43" s="5" t="s">
-        <v>19</v>
-      </c>
-      <c r="G43" s="5" t="s">
+      <c r="F43" s="18" t="s">
+        <v>19</v>
+      </c>
+      <c r="G43" s="18" t="s">
         <v>17</v>
       </c>
       <c r="H43" s="5" t="s">
         <v>18</v>
       </c>
-      <c r="I43" s="5" t="s">
-        <v>19</v>
-      </c>
-      <c r="J43" s="5" t="s">
+      <c r="I43" s="7" t="s">
+        <v>19</v>
+      </c>
+      <c r="J43" s="7" t="s">
         <v>17</v>
       </c>
       <c r="K43" s="5" t="s">
         <v>18</v>
       </c>
-      <c r="L43" s="5" t="s">
-        <v>19</v>
-      </c>
-      <c r="M43" s="5" t="s">
+      <c r="L43" s="7" t="s">
+        <v>19</v>
+      </c>
+      <c r="M43" s="7" t="s">
         <v>17</v>
       </c>
       <c r="P43" s="2" t="s">
@@ -3676,13 +3697,13 @@
       <c r="V43" s="9" t="s">
         <v>19</v>
       </c>
-      <c r="W43" s="5" t="s">
-        <v>18</v>
-      </c>
-      <c r="X43" s="11" t="s">
-        <v>17</v>
-      </c>
-      <c r="Y43" s="11" t="s">
+      <c r="W43" s="16" t="s">
+        <v>18</v>
+      </c>
+      <c r="X43" s="15" t="s">
+        <v>17</v>
+      </c>
+      <c r="Y43" s="15" t="s">
         <v>19</v>
       </c>
       <c r="Z43" s="5" t="s">
@@ -3699,37 +3720,37 @@
       <c r="A44" s="2" t="s">
         <v>5</v>
       </c>
-      <c r="B44" s="5" t="s">
-        <v>19</v>
-      </c>
-      <c r="C44" s="5" t="s">
+      <c r="B44" s="7" t="s">
+        <v>19</v>
+      </c>
+      <c r="C44" s="7" t="s">
         <v>17</v>
       </c>
       <c r="D44" s="5" t="s">
         <v>18</v>
       </c>
-      <c r="E44" s="5" t="s">
-        <v>19</v>
-      </c>
-      <c r="F44" s="5" t="s">
+      <c r="E44" s="18" t="s">
+        <v>19</v>
+      </c>
+      <c r="F44" s="18" t="s">
         <v>17</v>
       </c>
       <c r="G44" s="5" t="s">
         <v>18</v>
       </c>
-      <c r="H44" s="5" t="s">
-        <v>19</v>
-      </c>
-      <c r="I44" s="5" t="s">
+      <c r="H44" s="7" t="s">
+        <v>19</v>
+      </c>
+      <c r="I44" s="7" t="s">
         <v>17</v>
       </c>
       <c r="J44" s="5" t="s">
         <v>18</v>
       </c>
-      <c r="K44" s="5" t="s">
-        <v>19</v>
-      </c>
-      <c r="L44" s="5" t="s">
+      <c r="K44" s="7" t="s">
+        <v>19</v>
+      </c>
+      <c r="L44" s="7" t="s">
         <v>19</v>
       </c>
       <c r="M44" s="5" t="s">
@@ -3756,13 +3777,13 @@
       <c r="V44" s="5" t="s">
         <v>18</v>
       </c>
-      <c r="W44" s="11" t="s">
-        <v>17</v>
-      </c>
-      <c r="X44" s="11" t="s">
-        <v>19</v>
-      </c>
-      <c r="Y44" s="5" t="s">
+      <c r="W44" s="15" t="s">
+        <v>17</v>
+      </c>
+      <c r="X44" s="15" t="s">
+        <v>19</v>
+      </c>
+      <c r="Y44" s="16" t="s">
         <v>18</v>
       </c>
       <c r="Z44" s="7" t="s">
@@ -3779,40 +3800,40 @@
       <c r="A45" s="2" t="s">
         <v>6</v>
       </c>
-      <c r="B45" s="5" t="s">
-        <v>19</v>
-      </c>
-      <c r="C45" s="5" t="s">
+      <c r="B45" s="7" t="s">
+        <v>19</v>
+      </c>
+      <c r="C45" s="7" t="s">
         <v>17</v>
       </c>
       <c r="D45" s="5" t="s">
         <v>18</v>
       </c>
-      <c r="E45" s="5" t="s">
-        <v>19</v>
-      </c>
-      <c r="F45" s="5" t="s">
+      <c r="E45" s="18" t="s">
+        <v>19</v>
+      </c>
+      <c r="F45" s="18" t="s">
         <v>17</v>
       </c>
       <c r="G45" s="5" t="s">
         <v>18</v>
       </c>
-      <c r="H45" s="5" t="s">
-        <v>19</v>
-      </c>
-      <c r="I45" s="5" t="s">
+      <c r="H45" s="7" t="s">
+        <v>19</v>
+      </c>
+      <c r="I45" s="7" t="s">
         <v>17</v>
       </c>
       <c r="J45" s="5" t="s">
         <v>18</v>
       </c>
-      <c r="K45" s="5" t="s">
-        <v>19</v>
-      </c>
-      <c r="L45" s="5" t="s">
-        <v>19</v>
-      </c>
-      <c r="M45" s="5" t="s">
+      <c r="K45" s="7" t="s">
+        <v>19</v>
+      </c>
+      <c r="L45" s="7" t="s">
+        <v>19</v>
+      </c>
+      <c r="M45" s="14" t="s">
         <v>18</v>
       </c>
       <c r="P45" s="2" t="s">
@@ -3836,13 +3857,13 @@
       <c r="V45" s="5" t="s">
         <v>18</v>
       </c>
-      <c r="W45" s="11" t="s">
-        <v>17</v>
-      </c>
-      <c r="X45" s="11" t="s">
-        <v>19</v>
-      </c>
-      <c r="Y45" s="5" t="s">
+      <c r="W45" s="15" t="s">
+        <v>17</v>
+      </c>
+      <c r="X45" s="15" t="s">
+        <v>19</v>
+      </c>
+      <c r="Y45" s="16" t="s">
         <v>18</v>
       </c>
       <c r="Z45" s="7" t="s">
@@ -3851,7 +3872,7 @@
       <c r="AA45" s="7" t="s">
         <v>17</v>
       </c>
-      <c r="AB45" s="5" t="s">
+      <c r="AB45" s="17" t="s">
         <v>17</v>
       </c>
     </row>
@@ -3859,40 +3880,40 @@
       <c r="A46" s="2" t="s">
         <v>7</v>
       </c>
-      <c r="B46" s="5" t="s">
+      <c r="B46" s="7" t="s">
         <v>19</v>
       </c>
       <c r="C46" s="5" t="s">
         <v>18</v>
       </c>
-      <c r="D46" s="5" t="s">
-        <v>19</v>
-      </c>
-      <c r="E46" s="5" t="s">
+      <c r="D46" s="7" t="s">
+        <v>19</v>
+      </c>
+      <c r="E46" s="18" t="s">
         <v>17</v>
       </c>
       <c r="F46" s="5" t="s">
         <v>18</v>
       </c>
-      <c r="G46" s="5" t="s">
-        <v>19</v>
-      </c>
-      <c r="H46" s="5" t="s">
+      <c r="G46" s="18" t="s">
+        <v>19</v>
+      </c>
+      <c r="H46" s="7" t="s">
         <v>17</v>
       </c>
       <c r="I46" s="5" t="s">
         <v>18</v>
       </c>
-      <c r="J46" s="5" t="s">
-        <v>19</v>
-      </c>
-      <c r="K46" s="5" t="s">
+      <c r="J46" s="7" t="s">
+        <v>19</v>
+      </c>
+      <c r="K46" s="7" t="s">
         <v>17</v>
       </c>
       <c r="L46" s="5" t="s">
         <v>18</v>
       </c>
-      <c r="M46" s="5" t="s">
+      <c r="M46" s="18" t="s">
         <v>19</v>
       </c>
       <c r="P46" s="2" t="s">
@@ -3916,13 +3937,13 @@
       <c r="V46" s="9" t="s">
         <v>17</v>
       </c>
-      <c r="W46" s="11" t="s">
-        <v>19</v>
-      </c>
-      <c r="X46" s="5" t="s">
-        <v>18</v>
-      </c>
-      <c r="Y46" s="11" t="s">
+      <c r="W46" s="15" t="s">
+        <v>19</v>
+      </c>
+      <c r="X46" s="16" t="s">
+        <v>18</v>
+      </c>
+      <c r="Y46" s="15" t="s">
         <v>17</v>
       </c>
       <c r="Z46" s="7" t="s">
@@ -3931,7 +3952,7 @@
       <c r="AA46" s="5" t="s">
         <v>18</v>
       </c>
-      <c r="AB46" s="7" t="s">
+      <c r="AB46" s="13" t="s">
         <v>18</v>
       </c>
     </row>
@@ -3939,40 +3960,40 @@
       <c r="A47" s="2" t="s">
         <v>8</v>
       </c>
-      <c r="B47" s="5" t="s">
+      <c r="B47" s="7" t="s">
         <v>19</v>
       </c>
       <c r="C47" s="5" t="s">
         <v>18</v>
       </c>
-      <c r="D47" s="5" t="s">
-        <v>19</v>
-      </c>
-      <c r="E47" s="5" t="s">
+      <c r="D47" s="7" t="s">
+        <v>19</v>
+      </c>
+      <c r="E47" s="18" t="s">
         <v>17</v>
       </c>
       <c r="F47" s="5" t="s">
         <v>18</v>
       </c>
-      <c r="G47" s="5" t="s">
-        <v>19</v>
-      </c>
-      <c r="H47" s="5" t="s">
+      <c r="G47" s="18" t="s">
+        <v>19</v>
+      </c>
+      <c r="H47" s="7" t="s">
         <v>17</v>
       </c>
       <c r="I47" s="5" t="s">
         <v>18</v>
       </c>
-      <c r="J47" s="5" t="s">
-        <v>19</v>
-      </c>
-      <c r="K47" s="5" t="s">
+      <c r="J47" s="7" t="s">
+        <v>19</v>
+      </c>
+      <c r="K47" s="7" t="s">
         <v>17</v>
       </c>
       <c r="L47" s="5" t="s">
         <v>18</v>
       </c>
-      <c r="M47" s="5" t="s">
+      <c r="M47" s="7" t="s">
         <v>19</v>
       </c>
       <c r="P47" s="2" t="s">
@@ -3996,13 +4017,13 @@
       <c r="V47" s="9" t="s">
         <v>17</v>
       </c>
-      <c r="W47" s="11" t="s">
-        <v>19</v>
-      </c>
-      <c r="X47" s="5" t="s">
-        <v>18</v>
-      </c>
-      <c r="Y47" s="11" t="s">
+      <c r="W47" s="15" t="s">
+        <v>19</v>
+      </c>
+      <c r="X47" s="16" t="s">
+        <v>18</v>
+      </c>
+      <c r="Y47" s="15" t="s">
         <v>17</v>
       </c>
       <c r="Z47" s="7" t="s">
@@ -4017,5 +4038,6 @@
     </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+  <pageSetup orientation="portrait" horizontalDpi="0" verticalDpi="0"/>
 </worksheet>
 </file>
</xml_diff>